<commit_message>
Updated observation table format
</commit_message>
<xml_diff>
--- a/products/FCN/input.xlsx
+++ b/products/FCN/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TS Generator\Template-Generator\products\FCN Try\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\TS Generator\Template-Generator\TOOL\TS_Generator\products\FCN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54014CC7-753B-4872-9195-6AB36E0BB215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43070A9-FB0A-4F70-BD07-C5D34ABE01E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="163">
   <si>
     <t>Product</t>
   </si>
@@ -766,9 +766,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -804,6 +801,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1306,7 +1306,7 @@
         <f ca="1">B5</f>
         <v>10 March 2025</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>600000</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1331,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C74DF-B7C9-47E9-9B7B-A13599351EEC}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1342,22 +1342,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>34</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -1368,628 +1365,544 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14">
+      <c r="A2" s="13">
+        <f>IF(AND(B2&lt;&gt;"", C2&lt;&gt;"", D2&lt;&gt;""), MAX($A$1:A1)+1, "")</f>
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14" t="str">
+        <f>IF(H2="","",TEXT(H2,"dd mmmm yyyy"))</f>
+        <v>10 October 2024</v>
+      </c>
+      <c r="C2" s="14" t="str">
+        <f>IF(I2="","",TEXT(I2,"dd mmmm yyyy"))</f>
+        <v>18 October 2024</v>
+      </c>
+      <c r="D2" s="15">
+        <f t="shared" ref="D2:D24" si="0">IF(J2="","",J2)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="22">
         <v>45575</v>
       </c>
-      <c r="C2" s="15">
+      <c r="I2" s="9">
         <v>45583</v>
       </c>
-      <c r="D2" s="16">
+      <c r="J2" s="10">
         <v>1</v>
       </c>
-      <c r="G2" s="9">
-        <v>1</v>
-      </c>
-      <c r="H2" s="10">
-        <v>45575</v>
-      </c>
-      <c r="I2" s="10">
-        <v>45583</v>
-      </c>
-      <c r="J2" s="11">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
+        <f>IF(AND(B3&lt;&gt;"", C3&lt;&gt;"", D3&lt;&gt;""), MAX($A$1:A2)+1, "")</f>
         <v>2</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14" t="str">
+        <f t="shared" ref="B3:B25" si="1">IF(H3="","",TEXT(H3,"dd mmmm yyyy"))</f>
+        <v>11 November 2024</v>
+      </c>
+      <c r="C3" s="14" t="str">
+        <f t="shared" ref="C3:C25" si="2">IF(I3="","",TEXT(I3,"dd mmmm yyyy"))</f>
+        <v>18 November 2024</v>
+      </c>
+      <c r="D3" s="15">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="H3" s="22">
         <v>45607</v>
       </c>
-      <c r="C3" s="15">
+      <c r="I3" s="9">
         <v>45614</v>
       </c>
-      <c r="D3" s="16">
+      <c r="J3" s="10">
         <v>0.98</v>
       </c>
-      <c r="G3" s="9">
-        <v>2</v>
-      </c>
-      <c r="H3" s="10">
-        <v>45607</v>
-      </c>
-      <c r="I3" s="10">
-        <v>45614</v>
-      </c>
-      <c r="J3" s="11">
-        <v>0.98</v>
-      </c>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
+        <f>IF(AND(B4&lt;&gt;"", C4&lt;&gt;"", D4&lt;&gt;""), MAX($A$1:A3)+1, "")</f>
         <v>3</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>10 December 2024</v>
+      </c>
+      <c r="C4" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>17 December 2024</v>
+      </c>
+      <c r="D4" s="15">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+      <c r="H4" s="22">
         <v>45636</v>
       </c>
-      <c r="C4" s="15">
+      <c r="I4" s="9">
         <v>45643</v>
       </c>
-      <c r="D4" s="16">
+      <c r="J4" s="10">
         <v>0.96</v>
       </c>
-      <c r="G4" s="9">
-        <v>3</v>
-      </c>
-      <c r="H4" s="10">
-        <v>45636</v>
-      </c>
-      <c r="I4" s="10">
-        <v>45643</v>
-      </c>
-      <c r="J4" s="11">
-        <v>0.96</v>
-      </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
+        <f>IF(AND(B5&lt;&gt;"", C5&lt;&gt;"", D5&lt;&gt;""), MAX($A$1:A4)+1, "")</f>
         <v>4</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>10 January 2025</v>
+      </c>
+      <c r="C5" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>17 January 2025</v>
+      </c>
+      <c r="D5" s="15">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="H5" s="22">
         <v>45667</v>
       </c>
-      <c r="C5" s="15">
+      <c r="I5" s="9">
         <v>45674</v>
       </c>
-      <c r="D5" s="16">
+      <c r="J5" s="10">
         <v>0.94</v>
       </c>
-      <c r="G5" s="9">
-        <v>4</v>
-      </c>
-      <c r="H5" s="10">
-        <v>45667</v>
-      </c>
-      <c r="I5" s="10">
-        <v>45674</v>
-      </c>
-      <c r="J5" s="11">
-        <v>0.94</v>
-      </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
+        <f>IF(AND(B6&lt;&gt;"", C6&lt;&gt;"", D6&lt;&gt;""), MAX($A$1:A5)+1, "")</f>
         <v>5</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>10 February 2025</v>
+      </c>
+      <c r="C6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>18 February 2025</v>
+      </c>
+      <c r="D6" s="15">
+        <f t="shared" si="0"/>
+        <v>0.92</v>
+      </c>
+      <c r="H6" s="22">
         <v>45698</v>
       </c>
-      <c r="C6" s="15">
+      <c r="I6" s="9">
         <v>45706</v>
       </c>
-      <c r="D6" s="16">
+      <c r="J6" s="10">
         <v>0.92</v>
       </c>
-      <c r="G6" s="9">
-        <v>5</v>
-      </c>
-      <c r="H6" s="10">
-        <v>45698</v>
-      </c>
-      <c r="I6" s="10">
-        <v>45706</v>
-      </c>
-      <c r="J6" s="11">
-        <v>0.92</v>
-      </c>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
+        <f>IF(AND(B7&lt;&gt;"", C7&lt;&gt;"", D7&lt;&gt;""), MAX($A$1:A6)+1, "")</f>
         <v>6</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>10 March 2025</v>
+      </c>
+      <c r="C7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>17 March 2025</v>
+      </c>
+      <c r="D7" s="15">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="H7" s="22">
         <v>45726</v>
       </c>
-      <c r="C7" s="15">
+      <c r="I7" s="9">
         <v>45733</v>
       </c>
-      <c r="D7" s="16">
+      <c r="J7" s="10">
         <v>0.9</v>
       </c>
-      <c r="G7" s="9">
-        <v>6</v>
-      </c>
-      <c r="H7" s="10">
-        <v>45726</v>
-      </c>
-      <c r="I7" s="10">
-        <v>45733</v>
-      </c>
-      <c r="J7" s="11">
-        <v>0.9</v>
-      </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
-        <v>7</v>
-      </c>
-      <c r="B8" s="15">
-        <v>45757</v>
-      </c>
-      <c r="C8" s="15">
-        <v>45764</v>
-      </c>
-      <c r="D8" s="16">
-        <v>0.88</v>
-      </c>
-      <c r="G8" s="9">
-        <v>7</v>
-      </c>
-      <c r="H8" s="10">
-        <v>45757</v>
-      </c>
-      <c r="I8" s="10">
-        <v>45764</v>
-      </c>
-      <c r="J8" s="11">
-        <v>0.88</v>
-      </c>
+      <c r="A8" s="13" t="str">
+        <f>IF(AND(B8&lt;&gt;"", C8&lt;&gt;"", D8&lt;&gt;""), MAX($A$1:A7)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B8" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D8" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H8" s="22"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
-        <v>8</v>
-      </c>
-      <c r="B9" s="15">
-        <v>45789</v>
-      </c>
-      <c r="C9" s="15">
-        <v>45796</v>
-      </c>
-      <c r="D9" s="16">
-        <v>0.86</v>
-      </c>
-      <c r="G9" s="9">
-        <v>8</v>
-      </c>
-      <c r="H9" s="10">
-        <v>45789</v>
-      </c>
-      <c r="I9" s="10">
-        <v>45796</v>
-      </c>
-      <c r="J9" s="11">
-        <v>0.86</v>
-      </c>
+      <c r="A9" s="13" t="str">
+        <f>IF(AND(B9&lt;&gt;"", C9&lt;&gt;"", D9&lt;&gt;""), MAX($A$1:A8)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B9" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C9" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D9" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14">
-        <v>9</v>
-      </c>
-      <c r="B10" s="15">
-        <v>45818</v>
-      </c>
-      <c r="C10" s="15">
-        <v>45825</v>
-      </c>
-      <c r="D10" s="16">
-        <v>0.84</v>
-      </c>
-      <c r="G10" s="9">
-        <v>9</v>
-      </c>
-      <c r="H10" s="10">
-        <v>45818</v>
-      </c>
-      <c r="I10" s="10">
-        <v>45825</v>
-      </c>
-      <c r="J10" s="11">
-        <v>0.84</v>
-      </c>
+      <c r="A10" s="13" t="str">
+        <f>IF(AND(B10&lt;&gt;"", C10&lt;&gt;"", D10&lt;&gt;""), MAX($A$1:A9)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B10" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C10" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D10" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14">
-        <v>10</v>
-      </c>
-      <c r="B11" s="15">
-        <v>45848</v>
-      </c>
-      <c r="C11" s="15">
-        <v>45855</v>
-      </c>
-      <c r="D11" s="16">
-        <v>0.82</v>
-      </c>
-      <c r="G11" s="9">
-        <v>10</v>
-      </c>
-      <c r="H11" s="10">
-        <v>45848</v>
-      </c>
-      <c r="I11" s="10">
-        <v>45855</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0.82</v>
-      </c>
+      <c r="A11" s="13" t="str">
+        <f>IF(AND(B11&lt;&gt;"", C11&lt;&gt;"", D11&lt;&gt;""), MAX($A$1:A10)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B11" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C11" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D11" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H11" s="22"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14">
-        <v>11</v>
-      </c>
-      <c r="B12" s="15">
-        <v>45880</v>
-      </c>
-      <c r="C12" s="15">
-        <v>45887</v>
-      </c>
-      <c r="D12" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="G12" s="9">
-        <v>11</v>
-      </c>
-      <c r="H12" s="10">
-        <v>45880</v>
-      </c>
-      <c r="I12" s="10">
-        <v>45887</v>
-      </c>
-      <c r="J12" s="11">
-        <v>0.8</v>
-      </c>
+      <c r="A12" s="13" t="str">
+        <f>IF(AND(B12&lt;&gt;"", C12&lt;&gt;"", D12&lt;&gt;""), MAX($A$1:A11)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B12" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C12" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D12" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14">
-        <v>12</v>
-      </c>
-      <c r="B13" s="15">
-        <v>45575</v>
-      </c>
-      <c r="C13" s="15">
-        <v>45583</v>
-      </c>
-      <c r="D13" s="16">
-        <v>0.78</v>
-      </c>
-      <c r="G13" s="9">
-        <v>12</v>
-      </c>
-      <c r="H13" s="10">
-        <v>45575</v>
-      </c>
-      <c r="I13" s="10">
-        <v>45583</v>
-      </c>
-      <c r="J13" s="11">
-        <v>0.78</v>
-      </c>
+      <c r="A13" s="13" t="str">
+        <f>IF(AND(B13&lt;&gt;"", C13&lt;&gt;"", D13&lt;&gt;""), MAX($A$1:A12)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B13" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C13" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D13" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="15">
-        <v>45607</v>
-      </c>
-      <c r="C14" s="15">
-        <v>45614</v>
-      </c>
-      <c r="D14" s="16">
-        <v>0.76</v>
-      </c>
-      <c r="G14" s="9">
-        <v>13</v>
-      </c>
-      <c r="H14" s="10">
-        <v>45607</v>
-      </c>
-      <c r="I14" s="10">
-        <v>45614</v>
-      </c>
-      <c r="J14" s="11">
-        <v>0.76</v>
-      </c>
+      <c r="A14" s="13" t="str">
+        <f>IF(AND(B14&lt;&gt;"", C14&lt;&gt;"", D14&lt;&gt;""), MAX($A$1:A13)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B14" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C14" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D14" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H14" s="22"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14">
-        <v>14</v>
-      </c>
-      <c r="B15" s="15">
-        <v>45636</v>
-      </c>
-      <c r="C15" s="15">
-        <v>45643</v>
-      </c>
-      <c r="D15" s="16">
-        <v>0.74</v>
-      </c>
-      <c r="G15" s="9">
-        <v>14</v>
-      </c>
-      <c r="H15" s="10">
-        <v>45636</v>
-      </c>
-      <c r="I15" s="10">
-        <v>45643</v>
-      </c>
-      <c r="J15" s="11">
-        <v>0.74</v>
-      </c>
+      <c r="A15" s="13" t="str">
+        <f>IF(AND(B15&lt;&gt;"", C15&lt;&gt;"", D15&lt;&gt;""), MAX($A$1:A14)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B15" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C15" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D15" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
-        <v>15</v>
-      </c>
-      <c r="B16" s="15">
-        <v>45667</v>
-      </c>
-      <c r="C16" s="15">
-        <v>45674</v>
-      </c>
-      <c r="D16" s="16">
-        <v>0.72</v>
-      </c>
-      <c r="G16" s="9">
-        <v>15</v>
-      </c>
-      <c r="H16" s="10">
-        <v>45667</v>
-      </c>
-      <c r="I16" s="10">
-        <v>45674</v>
-      </c>
-      <c r="J16" s="11">
-        <v>0.72</v>
-      </c>
+      <c r="A16" s="13" t="str">
+        <f>IF(AND(B16&lt;&gt;"", C16&lt;&gt;"", D16&lt;&gt;""), MAX($A$1:A15)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B16" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C16" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D16" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14">
-        <v>16</v>
-      </c>
-      <c r="B17" s="15">
-        <v>45698</v>
-      </c>
-      <c r="C17" s="15">
-        <v>45706</v>
-      </c>
-      <c r="D17" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="G17" s="9">
-        <v>16</v>
-      </c>
-      <c r="H17" s="10">
-        <v>45698</v>
-      </c>
-      <c r="I17" s="10">
-        <v>45706</v>
-      </c>
-      <c r="J17" s="11">
-        <v>0.7</v>
-      </c>
+      <c r="A17" s="13" t="str">
+        <f>IF(AND(B17&lt;&gt;"", C17&lt;&gt;"", D17&lt;&gt;""), MAX($A$1:A16)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B17" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C17" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D17" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14">
-        <v>17</v>
-      </c>
-      <c r="B18" s="15">
-        <v>45726</v>
-      </c>
-      <c r="C18" s="15">
-        <v>45733</v>
-      </c>
-      <c r="D18" s="16">
-        <v>0.68</v>
-      </c>
-      <c r="G18" s="9">
-        <v>17</v>
-      </c>
-      <c r="H18" s="10">
-        <v>45726</v>
-      </c>
-      <c r="I18" s="10">
-        <v>45733</v>
-      </c>
-      <c r="J18" s="11">
-        <v>0.68</v>
-      </c>
+      <c r="A18" s="13" t="str">
+        <f>IF(AND(B18&lt;&gt;"", C18&lt;&gt;"", D18&lt;&gt;""), MAX($A$1:A17)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B18" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C18" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D18" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14">
-        <v>18</v>
-      </c>
-      <c r="B19" s="15">
-        <v>45607</v>
-      </c>
-      <c r="C19" s="15">
-        <v>45614</v>
-      </c>
-      <c r="D19" s="16">
-        <v>0.76</v>
-      </c>
-      <c r="G19" s="9">
-        <v>18</v>
-      </c>
-      <c r="H19" s="10">
-        <v>45607</v>
-      </c>
-      <c r="I19" s="10">
-        <v>45614</v>
-      </c>
-      <c r="J19" s="11">
-        <v>0.76</v>
-      </c>
+      <c r="A19" s="13" t="str">
+        <f>IF(AND(B19&lt;&gt;"", C19&lt;&gt;"", D19&lt;&gt;""), MAX($A$1:A18)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B19" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C19" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D19" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H19" s="22"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14">
-        <v>19</v>
-      </c>
-      <c r="B20" s="15">
-        <v>45636</v>
-      </c>
-      <c r="C20" s="15">
-        <v>45643</v>
-      </c>
-      <c r="D20" s="16">
-        <v>0.74</v>
-      </c>
-      <c r="G20" s="9">
-        <v>19</v>
-      </c>
-      <c r="H20" s="10">
-        <v>45636</v>
-      </c>
-      <c r="I20" s="10">
-        <v>45643</v>
-      </c>
-      <c r="J20" s="11">
-        <v>0.74</v>
-      </c>
+      <c r="A20" s="13" t="str">
+        <f>IF(AND(B20&lt;&gt;"", C20&lt;&gt;"", D20&lt;&gt;""), MAX($A$1:A19)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B20" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C20" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D20" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14">
-        <v>20</v>
-      </c>
-      <c r="B21" s="15">
-        <v>45575</v>
-      </c>
-      <c r="C21" s="15">
-        <v>45583</v>
-      </c>
-      <c r="D21" s="16">
-        <v>0.66035087719298302</v>
-      </c>
-      <c r="G21" s="9">
-        <v>20</v>
-      </c>
-      <c r="H21" s="10">
-        <v>45575</v>
-      </c>
-      <c r="I21" s="10">
-        <v>45583</v>
-      </c>
-      <c r="J21" s="11">
-        <v>0.66035087719298302</v>
-      </c>
+      <c r="A21" s="13" t="str">
+        <f>IF(AND(B21&lt;&gt;"", C21&lt;&gt;"", D21&lt;&gt;""), MAX($A$1:A20)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B21" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C21" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D21" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14">
-        <v>21</v>
-      </c>
-      <c r="B22" s="15">
-        <v>45607</v>
-      </c>
-      <c r="C22" s="15">
-        <v>45614</v>
-      </c>
-      <c r="D22" s="16">
-        <v>0.64333333333333398</v>
-      </c>
-      <c r="G22" s="9">
-        <v>21</v>
-      </c>
-      <c r="H22" s="10">
-        <v>45607</v>
-      </c>
-      <c r="I22" s="10">
-        <v>45614</v>
-      </c>
-      <c r="J22" s="11">
-        <v>0.64333333333333398</v>
-      </c>
+      <c r="A22" s="13" t="str">
+        <f>IF(AND(B22&lt;&gt;"", C22&lt;&gt;"", D22&lt;&gt;""), MAX($A$1:A21)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B22" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C22" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D22" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14">
-        <v>22</v>
-      </c>
-      <c r="B23" s="15">
-        <v>45636</v>
-      </c>
-      <c r="C23" s="15">
-        <v>45643</v>
-      </c>
-      <c r="D23" s="16">
-        <v>0.62631578947368405</v>
-      </c>
-      <c r="G23" s="9">
-        <v>22</v>
-      </c>
-      <c r="H23" s="10">
-        <v>45636</v>
-      </c>
-      <c r="I23" s="10">
-        <v>45643</v>
-      </c>
-      <c r="J23" s="11">
-        <v>0.62631578947368405</v>
-      </c>
+      <c r="A23" s="13" t="str">
+        <f>IF(AND(B23&lt;&gt;"", C23&lt;&gt;"", D23&lt;&gt;""), MAX($A$1:A22)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B23" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C23" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D23" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H23" s="22"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14">
-        <v>23</v>
-      </c>
-      <c r="B24" s="15">
-        <v>45667</v>
-      </c>
-      <c r="C24" s="15">
-        <v>45674</v>
-      </c>
-      <c r="D24" s="16">
-        <v>0.60929824561403501</v>
-      </c>
-      <c r="G24" s="9">
-        <v>23</v>
-      </c>
-      <c r="H24" s="10">
-        <v>45667</v>
-      </c>
-      <c r="I24" s="10">
-        <v>45674</v>
-      </c>
-      <c r="J24" s="11">
-        <v>0.60929824561403501</v>
-      </c>
+      <c r="A24" s="13" t="str">
+        <f>IF(AND(B24&lt;&gt;"", C24&lt;&gt;"", D24&lt;&gt;""), MAX($A$1:A23)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B24" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C24" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D24" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14">
-        <v>24</v>
-      </c>
-      <c r="B25" s="15">
-        <v>45698</v>
-      </c>
-      <c r="C25" s="15">
-        <v>45706</v>
-      </c>
-      <c r="D25" s="16">
-        <v>0.59228070175438596</v>
-      </c>
-      <c r="G25" s="9">
-        <v>24</v>
-      </c>
-      <c r="H25" s="10">
-        <v>45698</v>
-      </c>
-      <c r="I25" s="10">
-        <v>45706</v>
-      </c>
-      <c r="J25" s="11">
-        <v>0.59228070175438596</v>
-      </c>
+      <c r="A25" s="13" t="str">
+        <f>IF(AND(B25&lt;&gt;"", C25&lt;&gt;"", D25&lt;&gt;""), MAX($A$1:A24)+1, "")</f>
+        <v/>
+      </c>
+      <c r="B25" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C25" s="14" t="str">
+        <f>IF(I25="","",TEXT(I25,"dd mmmm yyyy"))</f>
+        <v/>
+      </c>
+      <c r="D25" s="15" t="str">
+        <f>IF(J25="","",J25)</f>
+        <v/>
+      </c>
+      <c r="H25" s="22"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2011,138 +1924,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="20" t="str">
+      <c r="H1" s="19" t="str">
         <f>IF('[1]Product Details'!D1="No EKI","Coupon Barrier Price","Knock-in Price")</f>
         <v>Coupon Barrier Price</v>
       </c>
-      <c r="I1" s="20" t="str">
+      <c r="I1" s="19" t="str">
         <f>IF('[1]Product Details'!D1="No EKI","","Coupon Barrier Price")</f>
         <v/>
       </c>
     </row>
     <row r="2" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="21">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="str">
+      <c r="B2" s="20" t="str">
         <f>VLOOKUP(C2,'BBG CODES'!A:D,2,FALSE)</f>
         <v>Alphabet Inc.</v>
       </c>
-      <c r="C2" s="22" t="str">
+      <c r="C2" s="21" t="str">
         <f>Main!D5</f>
         <v>GOOGL UQ</v>
       </c>
-      <c r="D2" s="22" t="str">
+      <c r="D2" s="21" t="str">
         <f>VLOOKUP(C2,'BBG CODES'!A:D,3,FALSE)</f>
         <v>NASDAQ Global Select Market</v>
       </c>
-      <c r="E2" s="22" t="str">
+      <c r="E2" s="21" t="str">
         <f>VLOOKUP(C2,'BBG CODES'!A:E,4,FALSE)</f>
         <v>USD</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="21">
+      <c r="A3" s="20">
         <f>IF(B3="","",A2+1)</f>
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="str">
+      <c r="B3" s="20" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C3,'BBG CODES'!A:D,2,FALSE),"")</f>
         <v>Amazon.com Inc.</v>
       </c>
-      <c r="C3" s="22" t="str">
+      <c r="C3" s="21" t="str">
         <f>Main!E5</f>
         <v>AMZN UQ</v>
       </c>
-      <c r="D3" s="22" t="str">
+      <c r="D3" s="21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C3,'BBG CODES'!A:D,3,FALSE),"")</f>
         <v>NASDAQ Global Select Market</v>
       </c>
-      <c r="E3" s="22" t="str">
+      <c r="E3" s="21" t="str">
         <f>VLOOKUP(C3,'BBG CODES'!A:E,4,FALSE)</f>
         <v>USD</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="str">
+      <c r="A4" s="20" t="str">
         <f>IF(B4="","",A3+1)</f>
         <v/>
       </c>
-      <c r="B4" s="21" t="str">
+      <c r="B4" s="20" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C4,'BBG CODES'!A:D,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="C4" s="22" t="str">
+      <c r="C4" s="21" t="str">
         <f>IF(Main!F5="","",Main!F5)</f>
         <v/>
       </c>
-      <c r="D4" s="22" t="str">
+      <c r="D4" s="21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C4,'BBG CODES'!A:D,3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="E4" s="22" t="str">
+      <c r="E4" s="21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C4,'BBG CODES'!A:E,4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="str">
+      <c r="A5" s="20" t="str">
         <f>IF(B5="","",A4+1)</f>
         <v/>
       </c>
-      <c r="B5" s="21" t="str">
+      <c r="B5" s="20" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C5,'BBG CODES'!A:D,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="C5" s="22" t="str">
+      <c r="C5" s="21" t="str">
         <f>IF(Main!G5="","",Main!G5)</f>
         <v/>
       </c>
-      <c r="D5" s="22" t="str">
+      <c r="D5" s="21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C5,'BBG CODES'!A:D,3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="E5" s="22" t="str">
+      <c r="E5" s="21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C5,'BBG CODES'!A:E,4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2153,20 +2066,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8423893D-5F5D-4D23-A981-AE5FA9F90797}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>